<commit_message>
Agregado un bit a la ALU
</commit_message>
<xml_diff>
--- a/Documentacion/TablaAlu_Nueva.xlsx
+++ b/Documentacion/TablaAlu_Nueva.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isaac Porras\Desktop\Decodification_ARM\Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skryf\Documents\Taller de Diseno Digital\Laboratorio 5\Decodification_ARM\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{791A6A6D-654C-4775-A59C-F0BB182C7C10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FEC4982-A7E5-4D5A-9E69-5579BE80FC33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{64B8AA29-57B9-4340-8CD9-D27D831A40FB}"/>
+    <workbookView xWindow="3600" yWindow="3660" windowWidth="21525" windowHeight="11385" xr2:uid="{64B8AA29-57B9-4340-8CD9-D27D831A40FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
   <si>
     <t>ALUOp</t>
   </si>
@@ -59,12 +59,6 @@
     <t>1</t>
   </si>
   <si>
-    <t>01</t>
-  </si>
-  <si>
-    <t>00</t>
-  </si>
-  <si>
     <t>1000</t>
   </si>
   <si>
@@ -89,10 +83,19 @@
     <t>1110</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>11</t>
+    <t>000</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>010</t>
+  </si>
+  <si>
+    <t>011</t>
+  </si>
+  <si>
+    <t>MOV</t>
   </si>
 </sst>
 </file>
@@ -160,13 +163,13 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -185,7 +188,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -484,61 +487,61 @@
   <dimension ref="D5:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="H17" sqref="H17:H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="5" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D11" s="6" t="s">
+    <row r="11" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D11" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="4" t="s">
         <v>4</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D12" s="3" t="s">
         <v>5</v>
       </c>
@@ -557,147 +560,158 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D13" s="4" t="s">
+    <row r="13" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D13" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>10</v>
+      <c r="E13" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" s="5" t="s">
+      <c r="G13" s="5" t="s">
         <v>9</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
+    <row r="14" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
       <c r="F14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="4"/>
-      <c r="H14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="6"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D15" s="4"/>
-      <c r="E15" s="5" t="s">
-        <v>13</v>
+    <row r="15" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D15" s="5"/>
+      <c r="E15" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G15" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>8</v>
+      <c r="G15" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D16" s="4"/>
-      <c r="E16" s="5"/>
+    <row r="16" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D16" s="5"/>
+      <c r="E16" s="6"/>
       <c r="F16" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G16" s="5"/>
-      <c r="H16" s="4"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="5"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D17" s="4"/>
-      <c r="E17" s="4" t="s">
-        <v>16</v>
+    <row r="17" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D17" s="5"/>
+      <c r="E17" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G17" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H17" s="5" t="s">
+      <c r="G17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" s="6" t="s">
         <v>18</v>
       </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
     </row>
-    <row r="18" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
+    <row r="18" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
       <c r="F18" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G18" s="4"/>
-      <c r="H18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="6"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D19" s="4"/>
-      <c r="E19" s="5" t="s">
-        <v>17</v>
+    <row r="19" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D19" s="5"/>
+      <c r="E19" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G19" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H19" s="4" t="s">
+      <c r="G19" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
-    <row r="20" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D20" s="4"/>
-      <c r="E20" s="5"/>
+    <row r="20" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D20" s="5"/>
+      <c r="E20" s="6"/>
       <c r="F20" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G20" s="5"/>
-      <c r="H20" s="4"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="5"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="G21" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="D13:D20"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="E19:E20"/>
     <mergeCell ref="G13:G14"/>
     <mergeCell ref="G15:G16"/>
     <mergeCell ref="G17:G18"/>
@@ -706,11 +720,6 @@
     <mergeCell ref="H15:H16"/>
     <mergeCell ref="H17:H18"/>
     <mergeCell ref="H19:H20"/>
-    <mergeCell ref="D13:D20"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="E19:E20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>